<commit_message>
docs: replace useless product backlog
</commit_message>
<xml_diff>
--- a/docs/Product Backlog-1.xlsx
+++ b/docs/Product Backlog-1.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamal\Desktop\Schoolwork\Summer 2025\ITSC 3155 (Software Engineering)\Group Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEE2CE0-DB5C-4E4B-BF4B-526C6C13CA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="14424" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>ITSC-3155 Software Engineering</t>
   </si>
@@ -31,19 +22,22 @@
     <t>Feature Name</t>
   </si>
   <si>
-    <t>PRIORITY</t>
-  </si>
-  <si>
-    <t>POINTS</t>
-  </si>
-  <si>
-    <t>DEFINE USER STORY</t>
-  </si>
-  <si>
-    <t>ASSIGNED TO SPRINT</t>
-  </si>
-  <si>
-    <t>SPRINT #</t>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>User Story</t>
+  </si>
+  <si>
+    <t>Assigned to Sprint</t>
+  </si>
+  <si>
+    <t>Sprint Number</t>
+  </si>
+  <si>
+    <t>Menu Item CRUD Operations</t>
   </si>
   <si>
     <t>High</t>
@@ -52,83 +46,180 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Online Ordering Interface</t>
-  </si>
-  <si>
-    <t>Develop customer-facing web/API platform</t>
-  </si>
-  <si>
-    <t>Enable guest checkout for new users</t>
-  </si>
-  <si>
-    <t>Design menu display with dish metadata</t>
-  </si>
-  <si>
-    <t>Provide takeout and delivery selection options</t>
-  </si>
-  <si>
-    <t>Integrate real-time order tracking system</t>
-  </si>
-  <si>
-    <t>Setup multi-method payment processing</t>
-  </si>
-  <si>
-    <t>Create role-based dashboards (staff/chef/admin)</t>
-  </si>
-  <si>
-    <t>Build real-time kitchen order display system</t>
-  </si>
-  <si>
-    <t>Develop admin analytics dashboard</t>
-  </si>
-  <si>
-    <t>Add customer review/rating module</t>
-  </si>
-  <si>
-    <t>Implement feedback reporting and analysis tools</t>
-  </si>
-  <si>
-    <t>Enable coupon and promo code engine</t>
-  </si>
-  <si>
-    <t>Build promotion management dashboard</t>
-  </si>
-  <si>
-    <t>Setup data analytics and sales reporting tools</t>
-  </si>
-  <si>
-    <t>Create integrated training resources for staff</t>
-  </si>
-  <si>
-    <t>Provide comprehensive system documentation repo</t>
-  </si>
-  <si>
-    <t>Medium</t>
+    <t>Menu Item Categories</t>
+  </si>
+  <si>
+    <t>Med</t>
+  </si>
+  <si>
+    <t>Menu Item Pricing &amp; Details</t>
+  </si>
+  <si>
+    <t>Menu Filtering System</t>
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>System to determine menu item availability</t>
+  </si>
+  <si>
+    <t>Resource/Ingredient System</t>
+  </si>
+  <si>
+    <t>Stock Updates</t>
+  </si>
+  <si>
+    <t>Availability Calculation</t>
+  </si>
+  <si>
+    <t>Recipe Creation</t>
+  </si>
+  <si>
+    <t>Guest Ordering (No Account Required)</t>
+  </si>
+  <si>
+    <t>Shopping Cart Functionality</t>
+  </si>
+  <si>
+    <t>Cart Item Management</t>
+  </si>
+  <si>
+    <t>Browser Session Management (order id)</t>
+  </si>
+  <si>
+    <t>Order Type Selection</t>
+  </si>
+  <si>
+    <t>Customer Information Collection</t>
+  </si>
+  <si>
+    <t>Menu Browsing</t>
+  </si>
+  <si>
+    <t>Order Creation &amp; Processing</t>
+  </si>
+  <si>
+    <t>Order Tracking Number System</t>
+  </si>
+  <si>
+    <t>Order Status Tracking</t>
+  </si>
+  <si>
+    <t>Order Validation</t>
+  </si>
+  <si>
+    <t>Order Status Management</t>
+  </si>
+  <si>
+    <t>Order Filtering by Status</t>
+  </si>
+  <si>
+    <t>Order Date Range Queries</t>
+  </si>
+  <si>
+    <t>Menu Item Creation</t>
+  </si>
+  <si>
+    <t>Inventory Management</t>
+  </si>
+  <si>
+    <t>Ingredient Requirements View</t>
+  </si>
+  <si>
+    <t>Promotion Code Creation</t>
+  </si>
+  <si>
+    <t>Promotion Management</t>
+  </si>
+  <si>
+    <t>Discount Application</t>
+  </si>
+  <si>
+    <t>Review System</t>
+  </si>
+  <si>
+    <t>Review Display</t>
+  </si>
+  <si>
+    <t>Review Management</t>
+  </si>
+  <si>
+    <t>Revenue Reporting</t>
+  </si>
+  <si>
+    <t>Dish Performance Analytics</t>
+  </si>
+  <si>
+    <t>Popularity Analytics</t>
+  </si>
+  <si>
+    <t>Review Analytics</t>
+  </si>
+  <si>
+    <t>Rating Analytics</t>
+  </si>
+  <si>
+    <t>Test Data Generation</t>
+  </si>
+  <si>
+    <t>Development Tools</t>
+  </si>
+  <si>
+    <t>Receipt Printing System</t>
+  </si>
+  <si>
+    <t>Restaurant Configuration</t>
+  </si>
+  <si>
+    <t>Tax Calculation</t>
+  </si>
+  <si>
+    <t>Receipt Formatting</t>
+  </si>
+  <si>
+    <t>Payment Processing</t>
+  </si>
+  <si>
+    <t>Checkout Process</t>
+  </si>
+  <si>
+    <t>Error Handling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="10"/>
-      <color indexed="12"/>
+      <color indexed="11"/>
       <name val="&quot;⋎ntury Gothic\&quot;&quot;"/>
     </font>
     <font>
@@ -137,7 +228,7 @@
       <name val="&quot;⋎ntury Gothic\&quot;&quot;"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,12 +249,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="8"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -272,97 +369,92 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="8"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
         <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -372,85 +464,26 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFF2CC"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="FFCFE2F3"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFBFBFBF"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="fffff2cc"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffcfe2f3"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -642,17 +675,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -670,19 +703,19 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -699,7 +732,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -724,7 +757,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -749,7 +782,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -774,7 +807,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -799,7 +832,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -824,7 +857,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -849,7 +882,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -874,7 +907,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -899,7 +932,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -912,32 +945,26 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -955,7 +982,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -980,7 +1007,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1005,7 +1032,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1030,7 +1057,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1055,7 +1082,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1080,7 +1107,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1105,7 +1132,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1130,7 +1157,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1155,7 +1182,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1180,7 +1207,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1193,15 +1220,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1215,7 +1236,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1233,19 +1254,19 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1262,7 +1283,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1287,7 +1308,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1312,7 +1333,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1337,7 +1358,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1362,7 +1383,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1387,7 +1408,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1412,7 +1433,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1437,7 +1458,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1462,7 +1483,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1475,419 +1496,990 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.44140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="12.44140625" style="1"/>
+    <col min="1" max="1" width="43.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="12.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A1" s="13" t="s">
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" t="s" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="10">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s" s="10">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s" s="10">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s" s="10">
         <v>6</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s" s="11">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="5" t="s">
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="12">
         <v>8</v>
       </c>
-      <c r="C4" s="6">
-        <v>8</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="B4" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="C4" s="13">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F5" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="14">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="F4" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1">
-      <c r="A5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="C6" s="13">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="12">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="C7" s="13">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F7" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C8" s="13">
         <v>5</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D8" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" t="s" s="12">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F9" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" t="s" s="12">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="F5" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
-      <c r="A6" s="7" t="s">
+      <c r="C10" s="13">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1">
+      <c r="A11" t="s" s="12">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="C11" s="13">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F11" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1">
+      <c r="A12" t="s" s="12">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="C12" s="13">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F12" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" ht="15" customHeight="1">
+      <c r="A13" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s" s="12">
         <v>12</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="8">
+      <c r="C13" s="13">
         <v>3</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D13" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F13" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1">
+      <c r="A14" t="s" s="12">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="C14" s="13">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F14" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1">
+      <c r="A15" t="s" s="12">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="F6" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1">
-      <c r="A7" s="7" t="s">
+      <c r="C15" s="13">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F15" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1">
+      <c r="A16" t="s" s="12">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="C16" s="13">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F16" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1">
+      <c r="A17" t="s" s="12">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="C17" s="13">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F17" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" t="s" s="12">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="C18" s="13">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F18" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" ht="15" customHeight="1">
+      <c r="A19" t="s" s="12">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C19" s="13">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F19" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" ht="15" customHeight="1">
+      <c r="A20" t="s" s="12">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="C20" s="13">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F20" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" ht="15" customHeight="1">
+      <c r="A21" t="s" s="12">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C21" s="13">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F21" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" ht="15" customHeight="1">
+      <c r="A22" t="s" s="12">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C22" s="13">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F22" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" ht="15" customHeight="1">
+      <c r="A23" t="s" s="12">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="C23" s="13">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F23" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" ht="15" customHeight="1">
+      <c r="A24" t="s" s="12">
+        <v>32</v>
+      </c>
+      <c r="B24" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C24" s="13">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F24" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" ht="15" customHeight="1">
+      <c r="A25" t="s" s="12">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="C25" s="13">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F25" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" ht="15" customHeight="1">
+      <c r="A26" t="s" s="12">
+        <v>34</v>
+      </c>
+      <c r="B26" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="C26" s="13">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F26" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" ht="15" customHeight="1">
+      <c r="A27" t="s" s="12">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="C27" s="13">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F27" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" ht="15" customHeight="1">
+      <c r="A28" t="s" s="12">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="C28" s="13">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F28" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" ht="15" customHeight="1">
+      <c r="A29" t="s" s="12">
+        <v>37</v>
+      </c>
+      <c r="B29" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="C29" s="13">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F29" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" ht="15" customHeight="1">
+      <c r="A30" t="s" s="12">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="C30" s="13">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E30" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F30" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" ht="15" customHeight="1">
+      <c r="A31" t="s" s="12">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="C31" s="13">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F31" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" ht="15" customHeight="1">
+      <c r="A32" t="s" s="12">
+        <v>40</v>
+      </c>
+      <c r="B32" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="C32" s="13">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E32" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F32" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" ht="15" customHeight="1">
+      <c r="A33" t="s" s="14">
+        <v>41</v>
+      </c>
+      <c r="B33" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C33" s="13">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F33" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" ht="15" customHeight="1">
+      <c r="A34" t="s" s="14">
+        <v>42</v>
+      </c>
+      <c r="B34" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C34" s="13">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F34" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" ht="15" customHeight="1">
+      <c r="A35" t="s" s="14">
+        <v>43</v>
+      </c>
+      <c r="B35" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C35" s="13">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F35" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" ht="15" customHeight="1">
+      <c r="A36" t="s" s="14">
+        <v>44</v>
+      </c>
+      <c r="B36" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C36" s="13">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E36" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F36" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" ht="15" customHeight="1">
+      <c r="A37" t="s" s="14">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C37" s="13">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F37" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" ht="15" customHeight="1">
+      <c r="A38" t="s" s="14">
+        <v>46</v>
+      </c>
+      <c r="B38" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C38" s="13">
+        <v>3</v>
+      </c>
+      <c r="D38" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E38" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F38" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" ht="15" customHeight="1">
+      <c r="A39" t="s" s="14">
+        <v>47</v>
+      </c>
+      <c r="B39" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="C39" s="13">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F39" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" ht="15" customHeight="1">
+      <c r="A40" t="s" s="14">
+        <v>48</v>
+      </c>
+      <c r="B40" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="C40" s="13">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F40" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" ht="15" customHeight="1">
+      <c r="A41" t="s" s="14">
+        <v>49</v>
+      </c>
+      <c r="B41" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C41" s="13">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F41" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" ht="15" customHeight="1">
+      <c r="A42" t="s" s="14">
+        <v>50</v>
+      </c>
+      <c r="B42" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C42" s="13">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F42" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" ht="15" customHeight="1">
+      <c r="A43" t="s" s="14">
+        <v>51</v>
+      </c>
+      <c r="B43" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="C43" s="13">
         <v>13</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="8">
-        <v>5</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="D43" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E43" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F43" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" ht="15" customHeight="1">
+      <c r="A44" t="s" s="14">
+        <v>52</v>
+      </c>
+      <c r="B44" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="C44" s="13">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E44" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F44" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" ht="15" customHeight="1">
+      <c r="A45" t="s" s="14">
+        <v>53</v>
+      </c>
+      <c r="B45" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="C45" s="13">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E45" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F45" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" ht="15" customHeight="1">
+      <c r="A46" t="s" s="14">
+        <v>54</v>
+      </c>
+      <c r="B46" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="C46" s="13">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E46" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F46" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" ht="15" customHeight="1">
+      <c r="A47" t="s" s="14">
+        <v>55</v>
+      </c>
+      <c r="B47" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="F7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1">
-      <c r="A8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="C47" s="13">
+        <v>13</v>
+      </c>
+      <c r="D47" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E47" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F47" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" ht="15" customHeight="1">
+      <c r="A48" t="s" s="14">
+        <v>56</v>
+      </c>
+      <c r="B48" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="C48" s="13">
         <v>3</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D48" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E48" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F48" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" ht="15" customHeight="1">
+      <c r="A49" t="s" s="14">
+        <v>57</v>
+      </c>
+      <c r="B49" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1">
-      <c r="A9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="8">
-        <v>8</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1">
-      <c r="A10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="8">
-        <v>8</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1">
-      <c r="A11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="8">
-        <v>8</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1">
-      <c r="A12" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="8">
-        <v>5</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1">
-      <c r="A13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="8">
-        <v>5</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1">
-      <c r="A14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="8">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1">
-      <c r="A15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="8">
-        <v>5</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1">
-      <c r="A16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="8">
-        <v>3</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1">
-      <c r="A17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="8">
-        <v>5</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1">
-      <c r="A18" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="8">
-        <v>8</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1">
-      <c r="A19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="8">
-        <v>2</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1">
-      <c r="A20" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="8">
-        <v>3</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="6">
+      <c r="C49" s="13">
+        <v>13</v>
+      </c>
+      <c r="D49" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="E49" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F49" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1896,16 +2488,8 @@
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B20" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"High,Medium,Low"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:E20" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>